<commit_message>
feat: update articles or snippets
</commit_message>
<xml_diff>
--- a/packages/excel-node-generator/src/__test__/test.xlsx
+++ b/packages/excel-node-generator/src/__test__/test.xlsx
@@ -7,14 +7,14 @@
     <sheet sheetId="1" name="发货单" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'发货单'!$A1:$J14</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'发货单'!$A1:$K14</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Unionfab AM Technology（Shanghai）Co.,Ltd</t>
   </si>
@@ -26,13 +26,184 @@
   </si>
   <si>
     <t>上海市松江区新格路 901 号 5 幢 3 楼</t>
+  </si>
+  <si>
+    <r>
+      <t>客户名称：</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+      </rPr>
+      <t xml:space="preserve">上海隽工自动化科技有限公司  </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>订单号：</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+      </rPr>
+      <t xml:space="preserve">XJ20201021-764483-2  </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>联系人：</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+      </rPr>
+      <t xml:space="preserve">方梦琪  </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>快递单号：</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+      </rPr>
+      <t xml:space="preserve">  </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>电话：</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+      </rPr>
+      <t xml:space="preserve">16602103254  </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>地址：</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+      </rPr>
+      <t xml:space="preserve">上海市松江区洞泾镇振业路280号1栋A8507室  </t>
+    </r>
+  </si>
+  <si>
+    <t>No.</t>
+  </si>
+  <si>
+    <t>文件名称</t>
+  </si>
+  <si>
+    <t>加工工艺</t>
+  </si>
+  <si>
+    <t>材料</t>
+  </si>
+  <si>
+    <t>增值后处理</t>
+  </si>
+  <si>
+    <t>数量（件）</t>
+  </si>
+  <si>
+    <t>备注</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>DSH-MCS-TO220-08-01-V1_Rescaled(9.99899)缩放.stl</t>
+  </si>
+  <si>
+    <t>SLA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">尼龙 </t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>注：若收货有差异或损耗，请于24小时内反馈至我司，过后视为正常签收；也可搜索 优联智造 微信小程序获取更多。</t>
+  </si>
+  <si>
+    <r>
+      <t>制单人：</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+      </rPr>
+      <t xml:space="preserve">  </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>发货人：</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+      </rPr>
+      <t xml:space="preserve">  </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>客户确认签章：</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+      </rPr>
+      <t xml:space="preserve">  </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>制单日期：</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+      </rPr>
+      <t>2020-10-21</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>发货日期：</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+      </rPr>
+      <t>2020-10-21</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>签收日期：</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+      </rPr>
+      <t>2020-10-21</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <color theme="1"/>
       <family val="2"/>
@@ -42,16 +213,19 @@
     </font>
     <font>
       <b/>
+      <sz val="12"/>
+    </font>
+    <font>
+      <b/>
       <sz val="16"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
+      <sz val="9"/>
     </font>
     <font>
       <b/>
-      <sz val="14"/>
     </font>
+    <font/>
   </fonts>
   <fills count="2">
     <fill>
@@ -61,7 +235,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -70,52 +244,104 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thick"/>
+      <left style="thin"/>
+      <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left/>
+      <right style="thin"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
       <right/>
       <top/>
-      <bottom style="thick"/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
     <border>
       <left/>
-      <right style="thick"/>
+      <right/>
       <top/>
-      <bottom style="thick"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin"/>
+      <top/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -188,9 +414,9 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -553,100 +779,229 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="20" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55" defaultColWidth="12" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="25" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55" defaultColWidth="12" customHeight="1"/>
   <cols>
     <col min="2" max="2" width="20" customWidth="1"/>
     <col min="3" max="3" width="1" customWidth="1"/>
-    <col min="4" max="5" width="8" customWidth="1"/>
+    <col min="4" max="4" width="10" customWidth="1"/>
+    <col min="5" max="5" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="25" customHeight="1" spans="6:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="F1" s="2" t="s">
+    <row r="1" ht="25" customHeight="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2"/>
+      <c r="F1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-    </row>
-    <row r="2" ht="30" customHeight="1" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+    </row>
+    <row r="2" ht="50" customHeight="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
       <c r="B2" s="1"/>
       <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-    </row>
-    <row r="3" ht="40" customHeight="1" spans="4:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="3" t="s">
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+    </row>
+    <row r="3" ht="30" customHeight="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="F3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-    </row>
-    <row r="4" spans="6:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="F4" s="4" t="s">
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+    </row>
+    <row r="4" ht="22.25" customHeight="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="F4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-    </row>
-    <row r="5" spans="10:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="J5" s="5"/>
-    </row>
-    <row r="6" spans="10:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="J6" s="5"/>
-    </row>
-    <row r="7" spans="10:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="J7" s="5"/>
-    </row>
-    <row r="8" spans="10:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="J8" s="5"/>
-    </row>
-    <row r="9" spans="10:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="J9" s="5"/>
-    </row>
-    <row r="10" spans="10:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="J10" s="5"/>
-    </row>
-    <row r="11" spans="10:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="J11" s="5"/>
-    </row>
-    <row r="12" spans="10:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="J12" s="5"/>
-    </row>
-    <row r="13" spans="10:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="J13" s="5"/>
-    </row>
-    <row r="14" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="6"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="7"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+    </row>
+    <row r="5" ht="11.25" customHeight="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="J5" s="6"/>
+    </row>
+    <row r="6" ht="22.25" customHeight="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="G6" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+    </row>
+    <row r="7" ht="22.25" customHeight="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="G7" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+    </row>
+    <row r="8" ht="22.25" customHeight="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="J8" s="6"/>
+    </row>
+    <row r="9" ht="22.25" customHeight="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="J9" s="6"/>
+    </row>
+    <row r="10" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+    </row>
+    <row r="12" ht="25" customHeight="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11"/>
+    </row>
+    <row r="13" ht="25" customHeight="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+    </row>
+    <row r="14" ht="25" customHeight="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="H14" s="15"/>
+      <c r="I14" s="15"/>
+      <c r="J14" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="23">
     <mergeCell ref="F1:J1"/>
-    <mergeCell ref="D2:E3"/>
     <mergeCell ref="F2:J2"/>
     <mergeCell ref="F3:J3"/>
     <mergeCell ref="F4:J4"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="G6:J6"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="G7:J7"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="A12:J12"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="G13:J13"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="G14:J14"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>